<commit_message>
Update Lista de Modelos Realizados.xlsx
</commit_message>
<xml_diff>
--- a/Lista de Modelos Realizados.xlsx
+++ b/Lista de Modelos Realizados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleja/Documents/Maestría Uniandes/Clases/Big Data y Machine Learning/Repositorios Git Hub/Problem_set_2_BDML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BFC730-F08B-0F42-95C5-CEE209D271DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B3FDDE-619B-424E-806E-B94DF6AA0471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28740" windowHeight="16020" xr2:uid="{062AE29A-9D6D-4AB4-820E-B2E0346F8EF5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Modelo</t>
   </si>
@@ -124,6 +124,31 @@
   </si>
   <si>
     <t>0.60</t>
+  </si>
+  <si>
+    <t>Ingtotug~Dominio + Depto + P5010 + 
+                      N_cuartos_hog + Nper + nmenores_5 + nmenores_6_11 + 
+                      nmenores_12_17 + nocupados + nincapacitados + ntrabajo_menores + 
+                      Head_Mujer + Head_Afiliado_SS + P5140 + Npersug +
+                      Head_exper_ult_trab + Head_Rec_alimento + Head_Rec_subsidio + 
+                      Head_Rec_vivienda + Head_Ocupacion + maxEducLevel + Head_Primas +
+                      Head_Segundo_trabajo + DormitorXpersona + Ln_Cuota + Head_Oficio +
+                      Ln_Pago_arrien + nmujeres + Ocup_vivienda + 
+                      Head_Cot_pension + Cabecera</t>
+  </si>
+  <si>
+    <t>XGBoosting</t>
+  </si>
+  <si>
+    <t>Ln_Ing_tot_hogar~Dominio + Depto + P5010 + 
+                        N_cuartos_hog + Nper + nmenores_5 + nmenores_6_11 + 
+                        nmenores_12_17 + nocupados + nincapacitados + ntrabajo_menores + 
+                        Head_Mujer + Head_Afiliado_SS + P5140 + Npersug +
+                        Head_exper_ult_trab + Head_Rec_alimento + Head_Rec_subsidio + 
+                        Head_Rec_vivienda + Head_Ocupacion + maxEducLevel + Head_Primas +
+                        Head_Segundo_trabajo + DormitorXpersona + Ln_Cuota + Head_Oficio +
+                        Ln_Pago_arrien + nmujeres + Ocup_vivienda + 
+                        Head_Cot_pension + Cabecera</t>
   </si>
 </sst>
 </file>
@@ -530,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54674CC-5F80-4ABC-822C-9614E6C2C51A}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -663,6 +688,28 @@
         <v>21</v>
       </c>
     </row>
+    <row r="10" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>